<commit_message>
STAYSL unfold of the simulated 88" with and without ETA.  Breakup in vault.
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
+++ b/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Radius [cm]</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Half-Life</t>
   </si>
   <si>
-    <t>Lambda</t>
-  </si>
-  <si>
     <t>AW</t>
   </si>
   <si>
@@ -183,7 +180,7 @@
     <t>σ (rel)</t>
   </si>
   <si>
-    <t>ENDF 115In(n,g)</t>
+    <t>Lambda [s^-1]</t>
   </si>
 </sst>
 </file>
@@ -255,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -358,9 +355,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -659,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,9 +673,10 @@
     <col min="14" max="14" width="8.88671875" style="11"/>
     <col min="15" max="15" width="8.88671875" style="6"/>
     <col min="16" max="16" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -689,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -700,8 +695,8 @@
       <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>50</v>
+      <c r="G1" s="55" t="s">
+        <v>49</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>0</v>
@@ -713,10 +708,10 @@
         <v>25</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>26</v>
@@ -725,13 +720,13 @@
         <v>27</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>8</v>
       </c>
@@ -748,7 +743,8 @@
         <v>9944835104.503521</v>
       </c>
       <c r="F2" s="40">
-        <v>5.4552099999999995E-7</v>
+        <f>0.000000545521*0.022148/0.02551</f>
+        <v>4.7362599404155227E-7</v>
       </c>
       <c r="G2" s="40">
         <v>4.4999999999999997E-3</v>
@@ -763,13 +759,13 @@
         <v>6.49</v>
       </c>
       <c r="K2" s="38">
-        <v>89.904700000000005</v>
+        <v>91.224000000000004</v>
       </c>
       <c r="L2" s="41">
         <v>0.51449999999999996</v>
       </c>
       <c r="M2" s="42">
-        <f t="shared" ref="M2:M20" si="0">3.141592654*H2^2*I2</f>
+        <f t="shared" ref="M2:M19" si="0">3.141592654*H2^2*I2</f>
         <v>1.9634954087500001</v>
       </c>
       <c r="N2" s="43">
@@ -777,15 +773,19 @@
         <v>282276</v>
       </c>
       <c r="O2" s="44">
-        <f t="shared" ref="O2:O20" si="1">0.6931471806/N2</f>
+        <f t="shared" ref="O2:O19" si="1">0.6931471806/N2</f>
         <v>2.4555654061981891E-6</v>
       </c>
       <c r="P2" s="44">
         <f>F2/(6.022E+23*J2/K2)/L2</f>
-        <v>2.4390631379007366E-29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2.1486902542385971E-29</v>
+      </c>
+      <c r="Q2">
+        <f>6.022*10^23*J2/K2*L2*10^-24</f>
+        <v>2.204254396869245E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>22</v>
       </c>
@@ -817,7 +817,7 @@
         <v>8.9079999999999995</v>
       </c>
       <c r="K3" s="42">
-        <v>57.935299999999998</v>
+        <v>58.693399999999997</v>
       </c>
       <c r="L3" s="48">
         <v>0.68076899999999996</v>
@@ -835,11 +835,15 @@
         <v>5.4084517837078655E-6</v>
       </c>
       <c r="P3" s="44">
-        <f t="shared" ref="P3:P20" si="2">F3/(6.022E+23*J3/K3)/L3</f>
-        <v>1.2163505477870959E-30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="P3:P19" si="2">F3/(6.022E+23*J3/K3)/L3</f>
+        <v>1.2322668432110842E-30</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q10" si="3">6.022*10^23*J3/K3*L3*10^-24</f>
+        <v>6.2220208571226059E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>13</v>
       </c>
@@ -871,7 +875,7 @@
         <v>8.9079999999999995</v>
       </c>
       <c r="K4" s="42">
-        <v>57.935299999999998</v>
+        <v>586934</v>
       </c>
       <c r="L4" s="48">
         <v>0.68076899999999996</v>
@@ -889,11 +893,15 @@
         <v>1.1321672046994073E-7</v>
       </c>
       <c r="P4" s="44">
-        <f t="shared" si="2"/>
-        <v>4.1753089198388224E-29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f>F4/(6.022E+23*J4/K4)/L4</f>
+        <v>4.2299440333556212E-25</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>6.222020857122606E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>19</v>
       </c>
@@ -925,7 +933,7 @@
         <v>7.31</v>
       </c>
       <c r="K5" s="38">
-        <v>114.9038</v>
+        <v>114.818</v>
       </c>
       <c r="L5" s="41">
         <v>0.95709999999999995</v>
@@ -943,11 +951,15 @@
         <v>4.2786863000000001E-5</v>
       </c>
       <c r="P5" s="44">
-        <f t="shared" si="2"/>
-        <v>2.0029656210806466E-29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <f>F5/(6.022E+23*J5/K5)/L5</f>
+        <v>2.0014699834229823E-29</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>3.6694879567663603E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>18</v>
       </c>
@@ -979,7 +991,7 @@
         <v>7.31</v>
       </c>
       <c r="K6" s="38">
-        <v>114.9038</v>
+        <v>114.818</v>
       </c>
       <c r="L6" s="41">
         <v>0.95709999999999995</v>
@@ -998,87 +1010,95 @@
       </c>
       <c r="P6" s="44">
         <f t="shared" si="2"/>
-        <v>1.8246332086852151E-30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1.8232707339080083E-30</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>3.6694879567663603E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C7" s="38">
-        <v>1293.56</v>
+        <v>355.7</v>
       </c>
       <c r="D7" s="38">
-        <v>84.8</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="E7" s="39">
         <v>9944835104.503521</v>
       </c>
       <c r="F7" s="40">
-        <v>8.2331400000000006E-8</v>
+        <v>4.4196E-6</v>
       </c>
       <c r="G7" s="40">
-        <v>3.7000000000000002E-3</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="H7" s="38">
         <v>2.5</v>
       </c>
       <c r="I7" s="38">
-        <v>0.1</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="J7" s="38">
-        <v>7.31</v>
+        <v>19.32</v>
       </c>
       <c r="K7" s="38">
-        <v>114.9038</v>
+        <v>196.9666</v>
       </c>
       <c r="L7" s="41">
-        <v>0.95709999999999995</v>
+        <v>1</v>
       </c>
       <c r="M7" s="42">
-        <f t="shared" ref="M7" si="3">3.141592654*H7^2*I7</f>
-        <v>1.9634954087500001</v>
+        <f t="shared" si="0"/>
+        <v>0.49872783382249997</v>
       </c>
       <c r="N7" s="43">
-        <f>54.12*60</f>
-        <v>3247.2</v>
+        <f>2.695*24*3600</f>
+        <v>232847.99999999997</v>
       </c>
       <c r="O7" s="44">
-        <f t="shared" ref="O7" si="4">0.6931471806/N7</f>
-        <v>2.134599595343681E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.9768225649350652E-6</v>
       </c>
       <c r="P7" s="44">
-        <f t="shared" ref="P7" si="5">F7/(6.022E+23*J7/K7)/L7</f>
-        <v>2.2453520688015329E-30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>7.4821718687792787E-29</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>5.9068410583317167E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="38">
-        <v>355.7</v>
+        <v>411.8</v>
       </c>
       <c r="D8" s="38">
-        <v>80.900000000000006</v>
+        <v>95.62</v>
       </c>
       <c r="E8" s="39">
         <v>9944835104.503521</v>
       </c>
       <c r="F8" s="40">
-        <v>4.4196E-6</v>
+        <v>6.5175E-8</v>
       </c>
       <c r="G8" s="40">
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="H8" s="38">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I8" s="38">
         <v>2.5399999999999999E-2</v>
@@ -1094,96 +1114,104 @@
       </c>
       <c r="M8" s="42">
         <f t="shared" si="0"/>
-        <v>0.31918581364639997</v>
+        <v>0.49872783382249997</v>
       </c>
       <c r="N8" s="43">
-        <f>2.695*24*3600</f>
-        <v>232847.99999999997</v>
+        <f>6.17*24*3600</f>
+        <v>533088</v>
       </c>
       <c r="O8" s="44">
         <f t="shared" si="1"/>
-        <v>2.9768225649350652E-6</v>
+        <v>1.3002490782009725E-6</v>
       </c>
       <c r="P8" s="44">
         <f t="shared" si="2"/>
-        <v>7.4821718687792787E-29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1.103381644374354E-30</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>5.9068410583317167E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="38">
-        <v>411.8</v>
-      </c>
-      <c r="D9" s="38">
-        <v>95.62</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="46">
+        <v>843.76</v>
+      </c>
+      <c r="D9" s="46">
+        <v>71.8</v>
       </c>
       <c r="E9" s="39">
         <v>9944835104.503521</v>
       </c>
-      <c r="F9" s="40">
-        <v>6.5175E-8</v>
-      </c>
-      <c r="G9" s="40">
-        <v>3.3999999999999998E-3</v>
+      <c r="F9" s="47">
+        <v>3.4033500000000001E-7</v>
+      </c>
+      <c r="G9" s="47">
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="H9" s="38">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I9" s="38">
-        <v>2.5399999999999999E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J9" s="38">
-        <v>19.32</v>
+        <v>2.7</v>
       </c>
       <c r="K9" s="38">
-        <v>196.9666</v>
+        <v>26.9815</v>
       </c>
       <c r="L9" s="41">
         <v>1</v>
       </c>
       <c r="M9" s="42">
         <f t="shared" si="0"/>
-        <v>0.31918581364639997</v>
+        <v>1.9634954087500001</v>
       </c>
       <c r="N9" s="43">
-        <f>6.17*24*3600</f>
-        <v>533088</v>
+        <f>9.458*60</f>
+        <v>567.48</v>
       </c>
       <c r="O9" s="44">
         <f t="shared" si="1"/>
-        <v>1.3002490782009725E-6</v>
+        <v>1.221447770141679E-3</v>
       </c>
       <c r="P9" s="44">
         <f t="shared" si="2"/>
-        <v>1.103381644374354E-30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>5.6476553885752242E-30</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>6.0261290143246306E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="46">
-        <v>843.76</v>
+        <v>1368.63</v>
       </c>
       <c r="D10" s="46">
-        <v>71.8</v>
+        <v>99.99</v>
       </c>
       <c r="E10" s="39">
         <v>9944835104.503521</v>
       </c>
       <c r="F10" s="47">
-        <v>3.4033500000000001E-7</v>
+        <v>3.1558700000000001E-7</v>
       </c>
       <c r="G10" s="47">
-        <v>2.7000000000000001E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="H10" s="38">
         <v>2.5</v>
@@ -1213,124 +1241,128 @@
         <v>1.28360589E-5</v>
       </c>
       <c r="P10" s="44">
+        <f>F10/(6.022E+23*J10/K10)/L10</f>
+        <v>5.2369771581362166E-30</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>6.0261290143246306E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="45">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F11" s="22">
+        <v>5.4645199999999996E-6</v>
+      </c>
+      <c r="G11" s="22">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="H11" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="J11" s="15">
+        <v>12.41</v>
+      </c>
+      <c r="K11" s="15">
+        <v>102.90560000000001</v>
+      </c>
+      <c r="L11" s="50">
+        <v>1</v>
+      </c>
+      <c r="M11" s="19">
+        <f t="shared" si="0"/>
+        <v>0.19634954087500001</v>
+      </c>
+      <c r="N11" s="51">
+        <f>56.114*60</f>
+        <v>3366.8399999999997</v>
+      </c>
+      <c r="O11" s="20">
+        <f t="shared" si="1"/>
+        <v>2.0587470167872547E-4</v>
+      </c>
+      <c r="P11" s="20">
         <f t="shared" si="2"/>
-        <v>5.6476553885752242E-30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="46">
-        <v>1368.63</v>
-      </c>
-      <c r="D11" s="46">
-        <v>99.99</v>
-      </c>
-      <c r="E11" s="39">
+        <v>7.5245147233712754E-29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="31">
+        <v>159.38</v>
+      </c>
+      <c r="D12" s="31">
+        <v>68.3</v>
+      </c>
+      <c r="E12" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F11" s="47">
-        <v>3.1558700000000001E-7</v>
-      </c>
-      <c r="G11" s="47">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="H11" s="38">
+      <c r="F12" s="32">
+        <v>1.3993199999999999E-8</v>
+      </c>
+      <c r="G12" s="32">
+        <v>5.3E-3</v>
+      </c>
+      <c r="H12" s="24">
         <v>2.5</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I12" s="24">
         <v>0.1</v>
       </c>
-      <c r="J11" s="38">
-        <v>2.7</v>
-      </c>
-      <c r="K11" s="38">
-        <v>26.9815</v>
-      </c>
-      <c r="L11" s="41">
-        <v>1</v>
-      </c>
-      <c r="M11" s="42">
+      <c r="J12" s="26">
+        <v>4.43</v>
+      </c>
+      <c r="K12" s="26">
+        <v>45.952599999999997</v>
+      </c>
+      <c r="L12" s="27">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="M12" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N11" s="50">
-        <f>114.74*24*3600</f>
-        <v>9913536</v>
-      </c>
-      <c r="O11" s="44">
+      <c r="N12" s="53">
+        <f>3.3492*24*3600</f>
+        <v>289370.88</v>
+      </c>
+      <c r="O12" s="30">
         <f t="shared" si="1"/>
-        <v>6.9919268018999477E-8</v>
-      </c>
-      <c r="P11" s="44">
-        <f>F11/(6.022E+23*J11/K11)/L11</f>
-        <v>5.2369771581362166E-30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="45">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F12" s="22">
-        <v>5.4645199999999996E-6</v>
-      </c>
-      <c r="G12" s="22">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="H12" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="J12" s="15">
-        <v>12.41</v>
-      </c>
-      <c r="K12" s="15">
-        <v>102.90560000000001</v>
-      </c>
-      <c r="L12" s="51">
-        <v>1</v>
-      </c>
-      <c r="M12" s="19">
-        <f t="shared" si="0"/>
-        <v>0.19634954087500001</v>
-      </c>
-      <c r="N12" s="52">
-        <f>56.114*60</f>
-        <v>3366.8399999999997</v>
-      </c>
-      <c r="O12" s="20">
-        <f t="shared" si="1"/>
-        <v>2.0587470167872547E-4</v>
-      </c>
-      <c r="P12" s="20">
-        <f t="shared" si="2"/>
-        <v>7.5245147233712754E-29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>2.3953591342708707E-6</v>
+      </c>
+      <c r="P12" s="30">
+        <f>F12/(6.022E+23*J12/K12)/L12</f>
+        <v>2.9216534713029442E-30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>36</v>
       </c>
       <c r="C13" s="31">
         <v>159.38</v>
@@ -1342,10 +1374,10 @@
         <v>9944835104.503521</v>
       </c>
       <c r="F13" s="32">
-        <v>1.3993199999999999E-8</v>
+        <v>3.83901E-8</v>
       </c>
       <c r="G13" s="32">
-        <v>5.3E-3</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="H13" s="24">
         <v>2.5</v>
@@ -1357,16 +1389,16 @@
         <v>4.43</v>
       </c>
       <c r="K13" s="26">
-        <v>45.952599999999997</v>
+        <v>46.951799999999999</v>
       </c>
       <c r="L13" s="27">
-        <v>8.2500000000000004E-2</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="M13" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N13" s="54">
+      <c r="N13" s="53">
         <f>3.3492*24*3600</f>
         <v>289370.88</v>
       </c>
@@ -1375,31 +1407,31 @@
         <v>2.3953591342708707E-6</v>
       </c>
       <c r="P13" s="30">
-        <f>F13/(6.022E+23*J13/K13)/L13</f>
-        <v>2.9216534713029442E-30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>9.0814265969195732E-30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="31">
-        <v>159.38</v>
+        <v>1312.12</v>
       </c>
       <c r="D14" s="31">
-        <v>68.3</v>
-      </c>
-      <c r="E14" s="25">
+        <v>100.1</v>
+      </c>
+      <c r="E14" s="35">
         <v>9944835104.503521</v>
       </c>
       <c r="F14" s="32">
-        <v>3.83901E-8</v>
+        <v>1.07354E-7</v>
       </c>
       <c r="G14" s="32">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H14" s="24">
         <v>2.5</v>
@@ -1407,107 +1439,107 @@
       <c r="I14" s="24">
         <v>0.1</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="24">
         <v>4.43</v>
       </c>
-      <c r="K14" s="26">
-        <v>46.951799999999999</v>
-      </c>
-      <c r="L14" s="27">
-        <v>7.4399999999999994E-2</v>
+      <c r="K14" s="24">
+        <v>47.947899999999997</v>
+      </c>
+      <c r="L14" s="36">
+        <v>0.73719999999999997</v>
       </c>
       <c r="M14" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="N14" s="54">
-        <f>3.3492*24*3600</f>
-        <v>289370.88</v>
+        <f>43.67*3600</f>
+        <v>157212</v>
       </c>
       <c r="O14" s="30">
         <f t="shared" si="1"/>
-        <v>2.3953591342708707E-6</v>
+        <v>4.4089966452942525E-6</v>
       </c>
       <c r="P14" s="30">
         <f t="shared" si="2"/>
-        <v>9.0814265969195732E-30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="31" t="s">
+        <v>2.6173271957228483E-30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="31">
-        <v>1312.12</v>
-      </c>
-      <c r="D15" s="31">
-        <v>100.1</v>
-      </c>
-      <c r="E15" s="35">
+      <c r="B15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="21">
+        <v>1761.9</v>
+      </c>
+      <c r="D15" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="16">
         <v>9944835104.503521</v>
       </c>
-      <c r="F15" s="32">
-        <v>1.07354E-7</v>
-      </c>
-      <c r="G15" s="32">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H15" s="24">
+      <c r="F15" s="22">
+        <v>5.3777699999999997E-9</v>
+      </c>
+      <c r="G15" s="22">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="H15" s="15">
         <v>2.5</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="15">
         <v>0.1</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="14">
         <v>4.43</v>
       </c>
-      <c r="K15" s="24">
-        <v>47.947899999999997</v>
-      </c>
-      <c r="L15" s="36">
-        <v>0.73719999999999997</v>
-      </c>
-      <c r="M15" s="28">
+      <c r="K15" s="17">
+        <v>48.947899999999997</v>
+      </c>
+      <c r="L15" s="18">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="M15" s="19">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N15" s="55">
-        <f>43.67*3600</f>
-        <v>157212</v>
-      </c>
-      <c r="O15" s="30">
+      <c r="N15" s="51">
+        <f>57.18*60</f>
+        <v>3430.8</v>
+      </c>
+      <c r="O15" s="20">
         <f t="shared" si="1"/>
-        <v>4.4089966452942525E-6</v>
-      </c>
-      <c r="P15" s="30">
+        <v>2.0203660388247639E-4</v>
+      </c>
+      <c r="P15" s="20">
         <f t="shared" si="2"/>
-        <v>2.6173271957228483E-30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1.8238727961479583E-30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" s="21">
-        <v>1761.9</v>
+        <v>1312.12</v>
       </c>
       <c r="D16" s="21">
-        <v>0.05</v>
+        <v>100.1</v>
       </c>
       <c r="E16" s="16">
         <v>9944835104.503521</v>
       </c>
       <c r="F16" s="22">
-        <v>5.3777699999999997E-9</v>
+        <v>9.1444600000000005E-10</v>
       </c>
       <c r="G16" s="22">
-        <v>3.2000000000000002E-3</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="H16" s="15">
         <v>2.5</v>
@@ -1529,93 +1561,93 @@
         <v>1.9634954087500001</v>
       </c>
       <c r="N16" s="52">
-        <f>57.18*60</f>
-        <v>3430.8</v>
+        <f>43.67*3600</f>
+        <v>157212</v>
       </c>
       <c r="O16" s="20">
         <f t="shared" si="1"/>
-        <v>2.0203660388247639E-4</v>
+        <v>4.4089966452942525E-6</v>
       </c>
       <c r="P16" s="20">
         <f t="shared" si="2"/>
-        <v>1.8238727961479583E-30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+        <v>3.101347180980808E-31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="21">
-        <v>1312.12</v>
-      </c>
-      <c r="D17" s="21">
-        <v>100.1</v>
-      </c>
-      <c r="E17" s="16">
+      <c r="B17" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="24">
+        <v>511</v>
+      </c>
+      <c r="D17" s="24">
+        <v>102</v>
+      </c>
+      <c r="E17" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F17" s="22">
-        <v>9.1444600000000005E-10</v>
-      </c>
-      <c r="G17" s="22">
-        <v>7.3000000000000001E-3</v>
-      </c>
-      <c r="H17" s="15">
+      <c r="F17" s="25">
+        <v>1.56262E-6</v>
+      </c>
+      <c r="G17" s="25">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="H17" s="24">
         <v>2.5</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="24">
         <v>0.1</v>
       </c>
-      <c r="J17" s="14">
-        <v>4.43</v>
-      </c>
-      <c r="K17" s="17">
-        <v>48.947899999999997</v>
-      </c>
-      <c r="L17" s="18">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="M17" s="19">
+      <c r="J17" s="24">
+        <v>6.77</v>
+      </c>
+      <c r="K17" s="26">
+        <v>140.90770000000001</v>
+      </c>
+      <c r="L17" s="27">
+        <v>1</v>
+      </c>
+      <c r="M17" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N17" s="53">
-        <f>43.67*3600</f>
-        <v>157212</v>
-      </c>
-      <c r="O17" s="20">
+      <c r="N17" s="29">
+        <f>3.39*60</f>
+        <v>203.4</v>
+      </c>
+      <c r="O17" s="30">
         <f t="shared" si="1"/>
-        <v>4.4089966452942525E-6</v>
-      </c>
-      <c r="P17" s="20">
+        <v>3.4078032477876108E-3</v>
+      </c>
+      <c r="P17" s="30">
         <f t="shared" si="2"/>
-        <v>3.101347180980808E-31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>5.4008073345541978E-29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="24">
+      <c r="B18" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="31">
         <v>511</v>
       </c>
-      <c r="D18" s="24">
-        <v>102</v>
+      <c r="D18" s="31">
+        <v>195.66</v>
       </c>
       <c r="E18" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F18" s="25">
-        <v>1.56262E-6</v>
-      </c>
-      <c r="G18" s="25">
-        <v>3.7000000000000002E-3</v>
+      <c r="F18" s="32">
+        <v>8.4934299999999998E-7</v>
+      </c>
+      <c r="G18" s="32">
+        <v>4.3E-3</v>
       </c>
       <c r="H18" s="24">
         <v>2.5</v>
@@ -1623,53 +1655,53 @@
       <c r="I18" s="24">
         <v>0.1</v>
       </c>
-      <c r="J18" s="24">
-        <v>6.77</v>
-      </c>
-      <c r="K18" s="26">
-        <v>140.90770000000001</v>
-      </c>
-      <c r="L18" s="27">
-        <v>1</v>
+      <c r="J18" s="26">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="K18" s="23">
+        <v>62.929600000000001</v>
+      </c>
+      <c r="L18" s="33">
+        <v>0.69169999999999998</v>
       </c>
       <c r="M18" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N18" s="29">
-        <f>3.39*60</f>
-        <v>203.4</v>
+      <c r="N18" s="34">
+        <f>9.673*60</f>
+        <v>580.38</v>
       </c>
       <c r="O18" s="30">
         <f t="shared" si="1"/>
-        <v>3.4078032477876108E-3</v>
+        <v>1.1942988741858783E-3</v>
       </c>
       <c r="P18" s="30">
         <f t="shared" si="2"/>
-        <v>5.4008073345541978E-29</v>
+        <v>1.4320940704440049E-29</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="31">
         <v>511</v>
       </c>
       <c r="D19" s="31">
-        <v>195.66</v>
+        <v>21.65</v>
       </c>
       <c r="E19" s="25">
         <v>9944835104.503521</v>
       </c>
       <c r="F19" s="32">
-        <v>8.4934299999999998E-7</v>
+        <v>6.81613E-7</v>
       </c>
       <c r="G19" s="32">
-        <v>4.3E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H19" s="24">
         <v>2.5</v>
@@ -1681,102 +1713,52 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="K19" s="23">
-        <v>62.929600000000001</v>
+        <v>64.927800000000005</v>
       </c>
       <c r="L19" s="33">
-        <v>0.69169999999999998</v>
+        <v>0.30830000000000002</v>
       </c>
       <c r="M19" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
       <c r="N19" s="34">
-        <f>9.673*60</f>
-        <v>580.38</v>
+        <f>12.701*3600</f>
+        <v>45723.6</v>
       </c>
       <c r="O19" s="30">
         <f t="shared" si="1"/>
-        <v>1.1942988741858783E-3</v>
+        <v>1.515950582631289E-5</v>
       </c>
       <c r="P19" s="30">
         <f t="shared" si="2"/>
-        <v>1.4320940704440049E-29</v>
+        <v>2.6603958818106171E-29</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="31">
-        <v>511</v>
-      </c>
-      <c r="D20" s="31">
-        <v>21.65</v>
-      </c>
-      <c r="E20" s="25">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F20" s="32">
-        <v>6.81613E-7</v>
-      </c>
-      <c r="G20" s="32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H20" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I20" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="J20" s="26">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="K20" s="23">
-        <v>64.927800000000005</v>
-      </c>
-      <c r="L20" s="33">
-        <v>0.30830000000000002</v>
-      </c>
-      <c r="M20" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9634954087500001</v>
-      </c>
-      <c r="N20" s="34">
-        <f>12.701*3600</f>
-        <v>45723.6</v>
-      </c>
-      <c r="O20" s="30">
-        <f t="shared" si="1"/>
-        <v>1.515950582631289E-5</v>
-      </c>
-      <c r="P20" s="30">
-        <f t="shared" si="2"/>
-        <v>2.6603958818106171E-29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="M21"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="M20"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I23" s="6"/>
       <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I25" s="6"/>
@@ -1889,10 +1871,6 @@
     <row r="52" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated STAYSL unfolding plots for Vault with ETA case. Updated Zr atom densities
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
+++ b/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
@@ -656,7 +656,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,10 +780,6 @@
         <f>F2/(6.022E+23*J2/K2)/L2</f>
         <v>2.1486902542385971E-29</v>
       </c>
-      <c r="Q2">
-        <f>6.022*10^23*J2/K2*L2*10^-24</f>
-        <v>2.204254396869245E-2</v>
-      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
@@ -838,10 +834,6 @@
         <f t="shared" ref="P3:P19" si="2">F3/(6.022E+23*J3/K3)/L3</f>
         <v>1.2322668432110842E-30</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q10" si="3">6.022*10^23*J3/K3*L3*10^-24</f>
-        <v>6.2220208571226059E-2</v>
-      </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
@@ -875,7 +867,7 @@
         <v>8.9079999999999995</v>
       </c>
       <c r="K4" s="42">
-        <v>586934</v>
+        <v>58.693399999999997</v>
       </c>
       <c r="L4" s="48">
         <v>0.68076899999999996</v>
@@ -894,12 +886,9 @@
       </c>
       <c r="P4" s="44">
         <f>F4/(6.022E+23*J4/K4)/L4</f>
-        <v>4.2299440333556212E-25</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="3"/>
-        <v>6.222020857122606E-6</v>
-      </c>
+        <v>4.2299440333556211E-29</v>
+      </c>
+      <c r="Q4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
@@ -954,10 +943,6 @@
         <f>F5/(6.022E+23*J5/K5)/L5</f>
         <v>2.0014699834229823E-29</v>
       </c>
-      <c r="Q5">
-        <f t="shared" si="3"/>
-        <v>3.6694879567663603E-2</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -1012,10 +997,6 @@
         <f t="shared" si="2"/>
         <v>1.8232707339080083E-30</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>3.6694879567663603E-2</v>
-      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
@@ -1070,10 +1051,6 @@
         <f t="shared" si="2"/>
         <v>7.4821718687792787E-29</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>5.9068410583317167E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
@@ -1128,10 +1105,6 @@
         <f t="shared" si="2"/>
         <v>1.103381644374354E-30</v>
       </c>
-      <c r="Q8">
-        <f t="shared" si="3"/>
-        <v>5.9068410583317167E-2</v>
-      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
@@ -1186,10 +1159,6 @@
         <f t="shared" si="2"/>
         <v>5.6476553885752242E-30</v>
       </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>6.0261290143246306E-2</v>
-      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
@@ -1243,10 +1212,6 @@
       <c r="P10" s="44">
         <f>F10/(6.022E+23*J10/K10)/L10</f>
         <v>5.2369771581362166E-30</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="3"/>
-        <v>6.0261290143246306E-2</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated 90Zr reaction rates to account for the error in atom density
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
+++ b/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Radius [cm]</t>
   </si>
@@ -123,15 +123,6 @@
     <t>Isotopic Fraction</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>103Rh(n,n')</t>
-  </si>
-  <si>
-    <t>103RhM</t>
-  </si>
-  <si>
     <t>46Ti(n,2n)</t>
   </si>
   <si>
@@ -154,12 +145,6 @@
   </si>
   <si>
     <t>49Ti(n,np)</t>
-  </si>
-  <si>
-    <t>141Pr(n,2n)</t>
-  </si>
-  <si>
-    <t>Pr140</t>
   </si>
   <si>
     <t>63Cu(n,2n)</t>
@@ -252,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -318,7 +303,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -346,7 +330,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -355,9 +338,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -653,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -695,8 +675,8 @@
       <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="55" t="s">
-        <v>49</v>
+      <c r="G1" s="52" t="s">
+        <v>44</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>0</v>
@@ -720,575 +700,575 @@
         <v>27</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="37">
         <v>909.15</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>99.04</v>
       </c>
-      <c r="E2" s="39">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F2" s="40">
+      <c r="E2" s="38">
+        <v>9944835104.5035191</v>
+      </c>
+      <c r="F2" s="39">
         <f>0.000000545521*0.022148/0.02551</f>
         <v>4.7362599404155227E-7</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="39">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="37">
         <v>2.5</v>
       </c>
-      <c r="I2" s="38">
+      <c r="I2" s="37">
         <v>0.1</v>
       </c>
-      <c r="J2" s="38">
+      <c r="J2" s="37">
         <v>6.49</v>
       </c>
-      <c r="K2" s="38">
+      <c r="K2" s="37">
         <v>91.224000000000004</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="40">
         <v>0.51449999999999996</v>
       </c>
-      <c r="M2" s="42">
-        <f t="shared" ref="M2:M19" si="0">3.141592654*H2^2*I2</f>
+      <c r="M2" s="41">
+        <f t="shared" ref="M2:M17" si="0">3.141592654*H2^2*I2</f>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N2" s="43">
+      <c r="N2" s="42">
         <f>78.41*3600</f>
         <v>282276</v>
       </c>
-      <c r="O2" s="44">
-        <f t="shared" ref="O2:O19" si="1">0.6931471806/N2</f>
+      <c r="O2" s="43">
+        <f t="shared" ref="O2:O17" si="1">0.6931471806/N2</f>
         <v>2.4555654061981891E-6</v>
       </c>
-      <c r="P2" s="44">
+      <c r="P2" s="43">
         <f>F2/(6.022E+23*J2/K2)/L2</f>
         <v>2.1486902542385971E-29</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="44">
         <v>1378</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="44">
         <v>81.7</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="45">
         <v>7.6671899999999995E-8</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="45">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="37">
         <v>2.5</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="37">
         <v>0.1</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="41">
         <v>8.9079999999999995</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="41">
         <v>58.693399999999997</v>
       </c>
-      <c r="L3" s="48">
+      <c r="L3" s="46">
         <v>0.68076899999999996</v>
       </c>
-      <c r="M3" s="42">
+      <c r="M3" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N3" s="49">
+      <c r="N3" s="47">
         <f>35.6*3600</f>
         <v>128160</v>
       </c>
-      <c r="O3" s="44">
+      <c r="O3" s="43">
         <f t="shared" si="1"/>
         <v>5.4084517837078655E-6</v>
       </c>
-      <c r="P3" s="44">
-        <f t="shared" ref="P3:P19" si="2">F3/(6.022E+23*J3/K3)/L3</f>
+      <c r="P3" s="43">
+        <f t="shared" ref="P3:P17" si="2">F3/(6.022E+23*J3/K3)/L3</f>
         <v>1.2322668432110842E-30</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="44">
         <v>810.76</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="44">
         <v>99.45</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="45">
         <v>2.63188E-6</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="45">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="37">
         <v>2.5</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="37">
         <v>0.1</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="36">
         <v>8.9079999999999995</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="41">
         <v>58.693399999999997</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="46">
         <v>0.68076899999999996</v>
       </c>
-      <c r="M4" s="42">
+      <c r="M4" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N4" s="49">
+      <c r="N4" s="47">
         <f>70.86*24*3600</f>
         <v>6122304</v>
       </c>
-      <c r="O4" s="44">
+      <c r="O4" s="43">
         <f t="shared" si="1"/>
         <v>1.1321672046994073E-7</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <f>F4/(6.022E+23*J4/K4)/L4</f>
         <v>4.2299440333556211E-29</v>
       </c>
       <c r="Q4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="37">
         <v>335</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <v>45.8</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="39">
         <v>7.3443699999999997E-7</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="45">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="37">
         <v>2.5</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="37">
         <v>0.1</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="37">
         <v>7.31</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="37">
         <v>114.818</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="40">
         <v>0.95709999999999995</v>
       </c>
-      <c r="M5" s="42">
+      <c r="M5" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="42">
         <f>4.5*3600</f>
         <v>16200</v>
       </c>
-      <c r="O5" s="44">
+      <c r="O5" s="43">
         <f t="shared" si="1"/>
         <v>4.2786863000000001E-5</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <f>F5/(6.022E+23*J5/K5)/L5</f>
         <v>2.0014699834229823E-29</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="37">
         <v>1293.56</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>84.8</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="39">
         <v>6.69047E-8</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="39">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="37">
         <v>2.5</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="37">
         <v>0.1</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="37">
         <v>7.31</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="37">
         <v>114.818</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="40">
         <v>0.95709999999999995</v>
       </c>
-      <c r="M6" s="42">
+      <c r="M6" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N6" s="43">
+      <c r="N6" s="42">
         <f>54.12*60</f>
         <v>3247.2</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="43">
         <f t="shared" si="1"/>
         <v>2.134599595343681E-4</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <f t="shared" si="2"/>
         <v>1.8232707339080083E-30</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="37">
         <v>355.7</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="37">
         <v>80.900000000000006</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="39">
         <v>4.4196E-6</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="39">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="37">
         <v>2.5</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="37">
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="37">
         <v>19.32</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7" s="37">
         <v>196.9666</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="40">
         <v>1</v>
       </c>
-      <c r="M7" s="42">
+      <c r="M7" s="41">
         <f t="shared" si="0"/>
         <v>0.49872783382249997</v>
       </c>
-      <c r="N7" s="43">
+      <c r="N7" s="42">
         <f>2.695*24*3600</f>
         <v>232847.99999999997</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="43">
         <f t="shared" si="1"/>
         <v>2.9768225649350652E-6</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <f t="shared" si="2"/>
         <v>7.4821718687792787E-29</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="37">
         <v>411.8</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="37">
         <v>95.62</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="39">
         <v>6.5175E-8</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="39">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="37">
         <v>2.5</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="37">
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="37">
         <v>19.32</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="37">
         <v>196.9666</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="40">
         <v>1</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="41">
         <f t="shared" si="0"/>
         <v>0.49872783382249997</v>
       </c>
-      <c r="N8" s="43">
+      <c r="N8" s="42">
         <f>6.17*24*3600</f>
         <v>533088</v>
       </c>
-      <c r="O8" s="44">
+      <c r="O8" s="43">
         <f t="shared" si="1"/>
         <v>1.3002490782009725E-6</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="43">
         <f t="shared" si="2"/>
         <v>1.103381644374354E-30</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="44">
         <v>843.76</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="44">
         <v>71.8</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="45">
         <v>3.4033500000000001E-7</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="45">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="37">
         <v>2.5</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="37">
         <v>0.1</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9" s="37">
         <v>2.7</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="37">
         <v>26.9815</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="40">
         <v>1</v>
       </c>
-      <c r="M9" s="42">
+      <c r="M9" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N9" s="43">
+      <c r="N9" s="42">
         <f>9.458*60</f>
         <v>567.48</v>
       </c>
-      <c r="O9" s="44">
+      <c r="O9" s="43">
         <f t="shared" si="1"/>
         <v>1.221447770141679E-3</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <f t="shared" si="2"/>
         <v>5.6476553885752242E-30</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="44">
         <v>1368.63</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="44">
         <v>99.99</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="38">
         <v>9944835104.503521</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="45">
         <v>3.1558700000000001E-7</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="45">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="37">
         <v>2.5</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="37">
         <v>0.1</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="37">
         <v>2.7</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="37">
         <v>26.9815</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="40">
         <v>1</v>
       </c>
-      <c r="M10" s="42">
+      <c r="M10" s="41">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="42">
         <f>15*3600</f>
         <v>54000</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="43">
         <f t="shared" si="1"/>
         <v>1.28360589E-5</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <f>F10/(6.022E+23*J10/K10)/L10</f>
         <v>5.2369771581362166E-30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="45">
+      <c r="C11" s="30">
+        <v>159.38</v>
+      </c>
+      <c r="D11" s="30">
+        <v>68.3</v>
+      </c>
+      <c r="E11" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F11" s="22">
-        <v>5.4645199999999996E-6</v>
-      </c>
-      <c r="G11" s="22">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="H11" s="15">
+      <c r="F11" s="31">
+        <v>1.3993199999999999E-8</v>
+      </c>
+      <c r="G11" s="31">
+        <v>5.3E-3</v>
+      </c>
+      <c r="H11" s="24">
         <v>2.5</v>
       </c>
-      <c r="I11" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="J11" s="15">
-        <v>12.41</v>
-      </c>
-      <c r="K11" s="15">
-        <v>102.90560000000001</v>
-      </c>
-      <c r="L11" s="50">
-        <v>1</v>
-      </c>
-      <c r="M11" s="19">
+      <c r="I11" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="26">
+        <v>4.43</v>
+      </c>
+      <c r="K11" s="26">
+        <v>45.952599999999997</v>
+      </c>
+      <c r="L11" s="27">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="M11" s="28">
         <f t="shared" si="0"/>
-        <v>0.19634954087500001</v>
-      </c>
-      <c r="N11" s="51">
-        <f>56.114*60</f>
-        <v>3366.8399999999997</v>
-      </c>
-      <c r="O11" s="20">
+        <v>1.9634954087500001</v>
+      </c>
+      <c r="N11" s="50">
+        <f>3.3492*24*3600</f>
+        <v>289370.88</v>
+      </c>
+      <c r="O11" s="29">
         <f t="shared" si="1"/>
-        <v>2.0587470167872547E-4</v>
-      </c>
-      <c r="P11" s="20">
-        <f t="shared" si="2"/>
-        <v>7.5245147233712754E-29</v>
+        <v>2.3953591342708707E-6</v>
+      </c>
+      <c r="P11" s="29">
+        <f>F11/(6.022E+23*J11/K11)/L11</f>
+        <v>2.9216534713029442E-30</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="31">
+        <v>33</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="30">
         <v>159.38</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>68.3</v>
       </c>
       <c r="E12" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F12" s="32">
-        <v>1.3993199999999999E-8</v>
-      </c>
-      <c r="G12" s="32">
-        <v>5.3E-3</v>
+      <c r="F12" s="31">
+        <v>3.83901E-8</v>
+      </c>
+      <c r="G12" s="31">
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="H12" s="24">
         <v>2.5</v>
@@ -1300,49 +1280,49 @@
         <v>4.43</v>
       </c>
       <c r="K12" s="26">
-        <v>45.952599999999997</v>
+        <v>46.951799999999999</v>
       </c>
       <c r="L12" s="27">
-        <v>8.2500000000000004E-2</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="M12" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N12" s="53">
+      <c r="N12" s="50">
         <f>3.3492*24*3600</f>
         <v>289370.88</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="29">
         <f t="shared" si="1"/>
         <v>2.3953591342708707E-6</v>
       </c>
-      <c r="P12" s="30">
-        <f>F12/(6.022E+23*J12/K12)/L12</f>
-        <v>2.9216534713029442E-30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="29">
+        <f t="shared" si="2"/>
+        <v>9.0814265969195732E-30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="31">
-        <v>159.38</v>
-      </c>
-      <c r="D13" s="31">
-        <v>68.3</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="C13" s="30">
+        <v>1312.12</v>
+      </c>
+      <c r="D13" s="30">
+        <v>100.1</v>
+      </c>
+      <c r="E13" s="34">
         <v>9944835104.503521</v>
       </c>
-      <c r="F13" s="32">
-        <v>3.83901E-8</v>
-      </c>
-      <c r="G13" s="32">
-        <v>2.5999999999999999E-3</v>
+      <c r="F13" s="31">
+        <v>1.07354E-7</v>
+      </c>
+      <c r="G13" s="31">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H13" s="24">
         <v>2.5</v>
@@ -1350,107 +1330,107 @@
       <c r="I13" s="24">
         <v>0.1</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="24">
         <v>4.43</v>
       </c>
-      <c r="K13" s="26">
-        <v>46.951799999999999</v>
-      </c>
-      <c r="L13" s="27">
-        <v>7.4399999999999994E-2</v>
+      <c r="K13" s="24">
+        <v>47.947899999999997</v>
+      </c>
+      <c r="L13" s="35">
+        <v>0.73719999999999997</v>
       </c>
       <c r="M13" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N13" s="53">
-        <f>3.3492*24*3600</f>
-        <v>289370.88</v>
-      </c>
-      <c r="O13" s="30">
+      <c r="N13" s="51">
+        <f>43.67*3600</f>
+        <v>157212</v>
+      </c>
+      <c r="O13" s="29">
         <f t="shared" si="1"/>
-        <v>2.3953591342708707E-6</v>
-      </c>
-      <c r="P13" s="30">
+        <v>4.4089966452942525E-6</v>
+      </c>
+      <c r="P13" s="29">
         <f t="shared" si="2"/>
-        <v>9.0814265969195732E-30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+        <v>2.6173271957228483E-30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="31">
-        <v>1312.12</v>
-      </c>
-      <c r="D14" s="31">
-        <v>100.1</v>
-      </c>
-      <c r="E14" s="35">
+      <c r="C14" s="21">
+        <v>1761.9</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="16">
         <v>9944835104.503521</v>
       </c>
-      <c r="F14" s="32">
-        <v>1.07354E-7</v>
-      </c>
-      <c r="G14" s="32">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H14" s="24">
+      <c r="F14" s="22">
+        <v>5.3777699999999997E-9</v>
+      </c>
+      <c r="G14" s="22">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="H14" s="15">
         <v>2.5</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="15">
         <v>0.1</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="14">
         <v>4.43</v>
       </c>
-      <c r="K14" s="24">
-        <v>47.947899999999997</v>
-      </c>
-      <c r="L14" s="36">
-        <v>0.73719999999999997</v>
-      </c>
-      <c r="M14" s="28">
+      <c r="K14" s="17">
+        <v>48.947899999999997</v>
+      </c>
+      <c r="L14" s="18">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="M14" s="19">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N14" s="54">
-        <f>43.67*3600</f>
-        <v>157212</v>
-      </c>
-      <c r="O14" s="30">
+      <c r="N14" s="48">
+        <f>57.18*60</f>
+        <v>3430.8</v>
+      </c>
+      <c r="O14" s="20">
         <f t="shared" si="1"/>
-        <v>4.4089966452942525E-6</v>
-      </c>
-      <c r="P14" s="30">
+        <v>2.0203660388247639E-4</v>
+      </c>
+      <c r="P14" s="20">
         <f t="shared" si="2"/>
-        <v>2.6173271957228483E-30</v>
+        <v>1.8238727961479583E-30</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C15" s="21">
-        <v>1761.9</v>
+        <v>1312.12</v>
       </c>
       <c r="D15" s="21">
-        <v>0.05</v>
+        <v>100.1</v>
       </c>
       <c r="E15" s="16">
         <v>9944835104.503521</v>
       </c>
       <c r="F15" s="22">
-        <v>5.3777699999999997E-9</v>
+        <v>9.1444600000000005E-10</v>
       </c>
       <c r="G15" s="22">
-        <v>3.2000000000000002E-3</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="H15" s="15">
         <v>2.5</v>
@@ -1471,94 +1451,94 @@
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N15" s="51">
-        <f>57.18*60</f>
-        <v>3430.8</v>
+      <c r="N15" s="49">
+        <f>43.67*3600</f>
+        <v>157212</v>
       </c>
       <c r="O15" s="20">
         <f t="shared" si="1"/>
-        <v>2.0203660388247639E-4</v>
+        <v>4.4089966452942525E-6</v>
       </c>
       <c r="P15" s="20">
         <f t="shared" si="2"/>
-        <v>1.8238727961479583E-30</v>
+        <v>3.101347180980808E-31</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="21">
-        <v>1312.12</v>
-      </c>
-      <c r="D16" s="21">
-        <v>100.1</v>
-      </c>
-      <c r="E16" s="16">
+      <c r="A16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="30">
+        <v>511</v>
+      </c>
+      <c r="D16" s="30">
+        <v>195.66</v>
+      </c>
+      <c r="E16" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F16" s="22">
-        <v>9.1444600000000005E-10</v>
-      </c>
-      <c r="G16" s="22">
-        <v>7.3000000000000001E-3</v>
-      </c>
-      <c r="H16" s="15">
+      <c r="F16" s="31">
+        <v>8.4934299999999998E-7</v>
+      </c>
+      <c r="G16" s="31">
+        <v>4.3E-3</v>
+      </c>
+      <c r="H16" s="24">
         <v>2.5</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="24">
         <v>0.1</v>
       </c>
-      <c r="J16" s="14">
-        <v>4.43</v>
-      </c>
-      <c r="K16" s="17">
-        <v>48.947899999999997</v>
-      </c>
-      <c r="L16" s="18">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="M16" s="19">
+      <c r="J16" s="26">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="K16" s="23">
+        <v>62.929600000000001</v>
+      </c>
+      <c r="L16" s="32">
+        <v>0.69169999999999998</v>
+      </c>
+      <c r="M16" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N16" s="52">
-        <f>43.67*3600</f>
-        <v>157212</v>
-      </c>
-      <c r="O16" s="20">
+      <c r="N16" s="33">
+        <f>9.673*60</f>
+        <v>580.38</v>
+      </c>
+      <c r="O16" s="29">
         <f t="shared" si="1"/>
-        <v>4.4089966452942525E-6</v>
-      </c>
-      <c r="P16" s="20">
+        <v>1.1942988741858783E-3</v>
+      </c>
+      <c r="P16" s="29">
         <f t="shared" si="2"/>
-        <v>3.101347180980808E-31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1.4320940704440049E-29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="24">
+      <c r="C17" s="30">
         <v>511</v>
       </c>
-      <c r="D17" s="24">
-        <v>102</v>
+      <c r="D17" s="30">
+        <v>21.65</v>
       </c>
       <c r="E17" s="25">
         <v>9944835104.503521</v>
       </c>
-      <c r="F17" s="25">
-        <v>1.56262E-6</v>
-      </c>
-      <c r="G17" s="25">
-        <v>3.7000000000000002E-3</v>
+      <c r="F17" s="31">
+        <v>6.81613E-7</v>
+      </c>
+      <c r="G17" s="31">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H17" s="24">
         <v>2.5</v>
@@ -1566,160 +1546,60 @@
       <c r="I17" s="24">
         <v>0.1</v>
       </c>
-      <c r="J17" s="24">
-        <v>6.77</v>
-      </c>
-      <c r="K17" s="26">
-        <v>140.90770000000001</v>
-      </c>
-      <c r="L17" s="27">
-        <v>1</v>
+      <c r="J17" s="26">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="K17" s="23">
+        <v>64.927800000000005</v>
+      </c>
+      <c r="L17" s="32">
+        <v>0.30830000000000002</v>
       </c>
       <c r="M17" s="28">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N17" s="29">
-        <f>3.39*60</f>
-        <v>203.4</v>
-      </c>
-      <c r="O17" s="30">
-        <f t="shared" si="1"/>
-        <v>3.4078032477876108E-3</v>
-      </c>
-      <c r="P17" s="30">
-        <f t="shared" si="2"/>
-        <v>5.4008073345541978E-29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="31">
-        <v>511</v>
-      </c>
-      <c r="D18" s="31">
-        <v>195.66</v>
-      </c>
-      <c r="E18" s="25">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F18" s="32">
-        <v>8.4934299999999998E-7</v>
-      </c>
-      <c r="G18" s="32">
-        <v>4.3E-3</v>
-      </c>
-      <c r="H18" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I18" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="J18" s="26">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="K18" s="23">
-        <v>62.929600000000001</v>
-      </c>
-      <c r="L18" s="33">
-        <v>0.69169999999999998</v>
-      </c>
-      <c r="M18" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9634954087500001</v>
-      </c>
-      <c r="N18" s="34">
-        <f>9.673*60</f>
-        <v>580.38</v>
-      </c>
-      <c r="O18" s="30">
-        <f t="shared" si="1"/>
-        <v>1.1942988741858783E-3</v>
-      </c>
-      <c r="P18" s="30">
-        <f t="shared" si="2"/>
-        <v>1.4320940704440049E-29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="31">
-        <v>511</v>
-      </c>
-      <c r="D19" s="31">
-        <v>21.65</v>
-      </c>
-      <c r="E19" s="25">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F19" s="32">
-        <v>6.81613E-7</v>
-      </c>
-      <c r="G19" s="32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H19" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I19" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="J19" s="26">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="K19" s="23">
-        <v>64.927800000000005</v>
-      </c>
-      <c r="L19" s="33">
-        <v>0.30830000000000002</v>
-      </c>
-      <c r="M19" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9634954087500001</v>
-      </c>
-      <c r="N19" s="34">
+      <c r="N17" s="33">
         <f>12.701*3600</f>
         <v>45723.6</v>
       </c>
-      <c r="O19" s="30">
+      <c r="O17" s="29">
         <f t="shared" si="1"/>
         <v>1.515950582631289E-5</v>
       </c>
-      <c r="P19" s="30">
+      <c r="P17" s="29">
         <f t="shared" si="2"/>
         <v>2.6603958818106171E-29</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="M20"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="7"/>
+    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="M18"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I24" s="6"/>
@@ -1728,6 +1608,10 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
+      <c r="L25">
+        <f>960+780+60+540</f>
+        <v>2340</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I26" s="6"/>
@@ -1828,14 +1712,6 @@
     <row r="50" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
-    </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated vault and ETA simulations and unfolds.  Minor changes to foil position, simulation cuts.  Added count plans.
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
+++ b/Simulated/88Inch_Activation/88_Vault/Foils.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Radius [cm]</t>
   </si>
@@ -138,12 +138,6 @@
     <t>Sc48</t>
   </si>
   <si>
-    <t>49Ti(n,p)</t>
-  </si>
-  <si>
-    <t>Sc49</t>
-  </si>
-  <si>
     <t>49Ti(n,np)</t>
   </si>
   <si>
@@ -166,6 +160,24 @@
   </si>
   <si>
     <t>Lambda [s^-1]</t>
+  </si>
+  <si>
+    <t>Ti45</t>
+  </si>
+  <si>
+    <t>46Ti(n,p)</t>
+  </si>
+  <si>
+    <t>Sc46</t>
+  </si>
+  <si>
+    <t>47Ti(n,np)</t>
+  </si>
+  <si>
+    <t>48Ti(n,np)</t>
+  </si>
+  <si>
+    <t>Count Time [s]</t>
   </si>
 </sst>
 </file>
@@ -199,18 +211,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -237,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -289,20 +295,22 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -310,49 +318,31 @@
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,7 +643,6 @@
     <col min="14" max="14" width="8.88671875" style="11"/>
     <col min="15" max="15" width="8.88671875" style="6"/>
     <col min="16" max="16" width="13.44140625" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -664,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -675,8 +664,8 @@
       <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="52" t="s">
-        <v>44</v>
+      <c r="G1" s="38" t="s">
+        <v>42</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>0</v>
@@ -700,683 +689,716 @@
         <v>27</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="Q1" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="25">
         <v>909.15</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="25">
         <v>99.04</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="26">
         <v>9944835104.5035191</v>
       </c>
-      <c r="F2" s="39">
-        <f>0.000000545521*0.022148/0.02551</f>
-        <v>4.7362599404155227E-7</v>
-      </c>
-      <c r="G2" s="39">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="H2" s="37">
+      <c r="F2" s="27">
+        <v>4.7166700000000001E-7</v>
+      </c>
+      <c r="G2" s="27">
+        <v>1.43E-2</v>
+      </c>
+      <c r="H2" s="25">
         <v>2.5</v>
       </c>
-      <c r="I2" s="37">
+      <c r="I2" s="25">
         <v>0.1</v>
       </c>
-      <c r="J2" s="37">
+      <c r="J2" s="25">
         <v>6.49</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="25">
         <v>91.224000000000004</v>
       </c>
-      <c r="L2" s="40">
+      <c r="L2" s="28">
         <v>0.51449999999999996</v>
       </c>
-      <c r="M2" s="41">
-        <f t="shared" ref="M2:M17" si="0">3.141592654*H2^2*I2</f>
+      <c r="M2" s="29">
+        <f t="shared" ref="M2:M19" si="0">3.141592654*H2^2*I2</f>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N2" s="42">
+      <c r="N2" s="30">
         <f>78.41*3600</f>
         <v>282276</v>
       </c>
-      <c r="O2" s="43">
-        <f t="shared" ref="O2:O17" si="1">0.6931471806/N2</f>
+      <c r="O2" s="31">
+        <f t="shared" ref="O2:O19" si="1">0.6931471806/N2</f>
         <v>2.4555654061981891E-6</v>
       </c>
-      <c r="P2" s="43">
+      <c r="P2" s="31">
         <f>F2/(6.022E+23*J2/K2)/L2</f>
-        <v>2.1486902542385971E-29</v>
+        <v>2.1398029223392721E-29</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="32">
         <v>1378</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="32">
         <v>81.7</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F3" s="45">
-        <v>7.6671899999999995E-8</v>
-      </c>
-      <c r="G3" s="45">
-        <v>4.7000000000000002E-3</v>
-      </c>
-      <c r="H3" s="37">
+      <c r="F3" s="33">
+        <v>7.6444000000000006E-8</v>
+      </c>
+      <c r="G3" s="33">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="H3" s="25">
         <v>2.5</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="25">
         <v>0.1</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="29">
         <v>8.9079999999999995</v>
       </c>
-      <c r="K3" s="41">
+      <c r="K3" s="29">
         <v>58.693399999999997</v>
       </c>
-      <c r="L3" s="46">
+      <c r="L3" s="34">
         <v>0.68076899999999996</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M3" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N3" s="47">
+      <c r="N3" s="35">
         <f>35.6*3600</f>
         <v>128160</v>
       </c>
-      <c r="O3" s="43">
+      <c r="O3" s="31">
         <f t="shared" si="1"/>
         <v>5.4084517837078655E-6</v>
       </c>
-      <c r="P3" s="43">
-        <f t="shared" ref="P3:P17" si="2">F3/(6.022E+23*J3/K3)/L3</f>
-        <v>1.2322668432110842E-30</v>
+      <c r="P3" s="31">
+        <f t="shared" ref="P3:P19" si="2">F3/(6.022E+23*J3/K3)/L3</f>
+        <v>1.2286040461033069E-30</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="32">
         <v>810.76</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="32">
         <v>99.45</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F4" s="45">
-        <v>2.63188E-6</v>
-      </c>
-      <c r="G4" s="45">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="H4" s="37">
+      <c r="F4" s="33">
+        <v>2.6581999999999998E-6</v>
+      </c>
+      <c r="G4" s="33">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="H4" s="25">
         <v>2.5</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="25">
         <v>0.1</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="24">
         <v>8.9079999999999995</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="29">
         <v>58.693399999999997</v>
       </c>
-      <c r="L4" s="46">
+      <c r="L4" s="34">
         <v>0.68076899999999996</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="35">
         <f>70.86*24*3600</f>
         <v>6122304</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="31">
         <f t="shared" si="1"/>
         <v>1.1321672046994073E-7</v>
       </c>
-      <c r="P4" s="43">
+      <c r="P4" s="31">
         <f>F4/(6.022E+23*J4/K4)/L4</f>
-        <v>4.2299440333556211E-29</v>
-      </c>
-      <c r="Q4"/>
+        <v>4.2722454023230208E-29</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>5000</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="25">
         <v>335</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="25">
         <v>45.8</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F5" s="39">
-        <v>7.3443699999999997E-7</v>
-      </c>
-      <c r="G5" s="45">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="H5" s="37">
+      <c r="F5" s="27">
+        <v>7.4170599999999998E-7</v>
+      </c>
+      <c r="G5" s="33">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="H5" s="25">
         <v>2.5</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="25">
         <v>0.1</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="25">
         <v>7.31</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="25">
         <v>114.818</v>
       </c>
-      <c r="L5" s="40">
+      <c r="L5" s="28">
         <v>0.95709999999999995</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N5" s="42">
+      <c r="N5" s="30">
         <f>4.5*3600</f>
         <v>16200</v>
       </c>
-      <c r="O5" s="43">
+      <c r="O5" s="31">
         <f t="shared" si="1"/>
         <v>4.2786863000000001E-5</v>
       </c>
-      <c r="P5" s="43">
+      <c r="P5" s="31">
         <f>F5/(6.022E+23*J5/K5)/L5</f>
-        <v>2.0014699834229823E-29</v>
+        <v>2.0212792867526097E-29</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="25">
         <v>1293.56</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="25">
         <v>84.8</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F6" s="39">
-        <v>6.69047E-8</v>
-      </c>
-      <c r="G6" s="39">
-        <v>3.7000000000000002E-3</v>
-      </c>
-      <c r="H6" s="37">
+      <c r="F6" s="27">
+        <v>6.7515500000000007E-8</v>
+      </c>
+      <c r="G6" s="27">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="H6" s="25">
         <v>2.5</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="25">
         <v>0.1</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="25">
         <v>7.31</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="25">
         <v>114.818</v>
       </c>
-      <c r="L6" s="40">
+      <c r="L6" s="28">
         <v>0.95709999999999995</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N6" s="42">
+      <c r="N6" s="30">
         <f>54.12*60</f>
         <v>3247.2</v>
       </c>
-      <c r="O6" s="43">
+      <c r="O6" s="31">
         <f t="shared" si="1"/>
         <v>2.134599595343681E-4</v>
       </c>
-      <c r="P6" s="43">
+      <c r="P6" s="31">
         <f t="shared" si="2"/>
-        <v>1.8232707339080083E-30</v>
+        <v>1.839916108063651E-30</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>750</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="25">
         <v>355.7</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="25">
         <v>80.900000000000006</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F7" s="39">
-        <v>4.4196E-6</v>
-      </c>
-      <c r="G7" s="39">
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="H7" s="37">
+      <c r="F7" s="27">
+        <v>4.4659199999999996E-6</v>
+      </c>
+      <c r="G7" s="27">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="H7" s="25">
         <v>2.5</v>
       </c>
-      <c r="I7" s="37">
-        <v>2.5399999999999999E-2</v>
-      </c>
-      <c r="J7" s="37">
+      <c r="I7" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="25">
         <v>19.32</v>
       </c>
-      <c r="K7" s="37">
+      <c r="K7" s="25">
         <v>196.9666</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="28">
         <v>1</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="29">
         <f t="shared" si="0"/>
-        <v>0.49872783382249997</v>
-      </c>
-      <c r="N7" s="42">
+        <v>0.19634954087500001</v>
+      </c>
+      <c r="N7" s="30">
+        <f>6.17*24*3600</f>
+        <v>533088</v>
+      </c>
+      <c r="O7" s="31">
+        <f t="shared" si="1"/>
+        <v>1.3002490782009725E-6</v>
+      </c>
+      <c r="P7" s="31">
+        <f>F7/(6.022E+23*J7/K7)/L7</f>
+        <v>7.5605894180963785E-29</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25">
+        <v>411.8</v>
+      </c>
+      <c r="D8" s="25">
+        <v>95.62</v>
+      </c>
+      <c r="E8" s="26">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F8" s="27">
+        <v>7.6984600000000002E-8</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1.26E-2</v>
+      </c>
+      <c r="H8" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="J8" s="25">
+        <v>19.32</v>
+      </c>
+      <c r="K8" s="25">
+        <v>196.9666</v>
+      </c>
+      <c r="L8" s="28">
+        <v>1</v>
+      </c>
+      <c r="M8" s="29">
+        <f t="shared" si="0"/>
+        <v>0.19634954087500001</v>
+      </c>
+      <c r="N8" s="30">
         <f>2.695*24*3600</f>
         <v>232847.99999999997</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O8" s="31">
         <f t="shared" si="1"/>
         <v>2.9768225649350652E-6</v>
       </c>
-      <c r="P7" s="43">
+      <c r="P8" s="31">
         <f t="shared" si="2"/>
-        <v>7.4821718687792787E-29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="37">
-        <v>411.8</v>
-      </c>
-      <c r="D8" s="37">
-        <v>95.62</v>
-      </c>
-      <c r="E8" s="38">
+        <v>1.3033125360874858E-30</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>18780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="32">
+        <v>843.76</v>
+      </c>
+      <c r="D9" s="32">
+        <v>71.8</v>
+      </c>
+      <c r="E9" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F8" s="39">
-        <v>6.5175E-8</v>
-      </c>
-      <c r="G8" s="39">
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="H8" s="37">
+      <c r="F9" s="33">
+        <v>3.4659199999999998E-7</v>
+      </c>
+      <c r="G9" s="33">
+        <v>8.6E-3</v>
+      </c>
+      <c r="H9" s="25">
         <v>2.5</v>
       </c>
-      <c r="I8" s="37">
-        <v>2.5399999999999999E-2</v>
-      </c>
-      <c r="J8" s="37">
-        <v>19.32</v>
-      </c>
-      <c r="K8" s="37">
-        <v>196.9666</v>
-      </c>
-      <c r="L8" s="40">
+      <c r="I9" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="25">
+        <v>2.7</v>
+      </c>
+      <c r="K9" s="25">
+        <v>26.9815</v>
+      </c>
+      <c r="L9" s="28">
         <v>1</v>
       </c>
-      <c r="M8" s="41">
-        <f t="shared" si="0"/>
-        <v>0.49872783382249997</v>
-      </c>
-      <c r="N8" s="42">
-        <f>6.17*24*3600</f>
-        <v>533088</v>
-      </c>
-      <c r="O8" s="43">
-        <f t="shared" si="1"/>
-        <v>1.3002490782009725E-6</v>
-      </c>
-      <c r="P8" s="43">
-        <f t="shared" si="2"/>
-        <v>1.103381644374354E-30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="44">
-        <v>843.76</v>
-      </c>
-      <c r="D9" s="44">
-        <v>71.8</v>
-      </c>
-      <c r="E9" s="38">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F9" s="45">
-        <v>3.4033500000000001E-7</v>
-      </c>
-      <c r="G9" s="45">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="H9" s="37">
-        <v>2.5</v>
-      </c>
-      <c r="I9" s="37">
-        <v>0.1</v>
-      </c>
-      <c r="J9" s="37">
-        <v>2.7</v>
-      </c>
-      <c r="K9" s="37">
-        <v>26.9815</v>
-      </c>
-      <c r="L9" s="40">
-        <v>1</v>
-      </c>
-      <c r="M9" s="41">
+      <c r="M9" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N9" s="42">
+      <c r="N9" s="30">
         <f>9.458*60</f>
         <v>567.48</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="31">
         <f t="shared" si="1"/>
         <v>1.221447770141679E-3</v>
       </c>
-      <c r="P9" s="43">
+      <c r="P9" s="31">
         <f t="shared" si="2"/>
-        <v>5.6476553885752242E-30</v>
+        <v>5.7514865542393935E-30</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="32">
         <v>1368.63</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="32">
         <v>99.99</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F10" s="45">
-        <v>3.1558700000000001E-7</v>
-      </c>
-      <c r="G10" s="45">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="H10" s="37">
+      <c r="F10" s="33">
+        <v>3.2046E-7</v>
+      </c>
+      <c r="G10" s="33">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="H10" s="25">
         <v>2.5</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="25">
         <v>0.1</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="25">
         <v>2.7</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="25">
         <v>26.9815</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="28">
         <v>1</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N10" s="42">
+      <c r="N10" s="30">
         <f>15*3600</f>
         <v>54000</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="31">
         <f t="shared" si="1"/>
         <v>1.28360589E-5</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="31">
         <f>F10/(6.022E+23*J10/K10)/L10</f>
-        <v>5.2369771581362166E-30</v>
+        <v>5.3178416731244699E-30</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="30">
-        <v>159.38</v>
-      </c>
-      <c r="D11" s="30">
-        <v>68.3</v>
-      </c>
-      <c r="E11" s="25">
+      <c r="B11" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="32">
+        <v>511</v>
+      </c>
+      <c r="D11" s="32">
+        <v>169.6</v>
+      </c>
+      <c r="E11" s="27">
         <v>9944835104.503521</v>
       </c>
-      <c r="F11" s="31">
-        <v>1.3993199999999999E-8</v>
-      </c>
-      <c r="G11" s="31">
-        <v>5.3E-3</v>
-      </c>
-      <c r="H11" s="24">
+      <c r="F11" s="33">
+        <v>1.3239899999999999E-8</v>
+      </c>
+      <c r="G11" s="33">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="H11" s="25">
         <v>2.5</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="25">
         <v>0.1</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="39">
         <v>4.43</v>
       </c>
-      <c r="K11" s="26">
-        <v>45.952599999999997</v>
-      </c>
-      <c r="L11" s="27">
+      <c r="K11" s="39">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L11" s="42">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="M11" s="28">
+      <c r="M11" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N11" s="50">
+      <c r="N11" s="43">
+        <v>11088</v>
+      </c>
+      <c r="O11" s="31">
+        <f t="shared" si="1"/>
+        <v>6.2513273863636361E-5</v>
+      </c>
+      <c r="P11" s="31">
+        <f>F11/(6.022E+23*J11/K11)/L11</f>
+        <v>2.8795358410501526E-30</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="21">
+        <v>889.27700000000004</v>
+      </c>
+      <c r="D12" s="21">
+        <v>99.983999999999995</v>
+      </c>
+      <c r="E12" s="16">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F12" s="22">
+        <v>8.0956300000000003E-8</v>
+      </c>
+      <c r="G12" s="22">
+        <v>8.6E-3</v>
+      </c>
+      <c r="H12" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="I12" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="17">
+        <v>4.43</v>
+      </c>
+      <c r="K12" s="17">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L12" s="18">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="M12" s="19">
+        <f t="shared" ref="M12" si="3">3.141592654*H12^2*I12</f>
+        <v>1.9634954087500001</v>
+      </c>
+      <c r="N12" s="36">
+        <v>7239456.0000000009</v>
+      </c>
+      <c r="O12" s="20">
+        <f t="shared" ref="O12" si="4">0.6931471806/N12</f>
+        <v>9.5745755012531324E-8</v>
+      </c>
+      <c r="P12" s="20">
+        <f t="shared" ref="P12" si="5">F12/(6.022E+23*J12/K12)/L12</f>
+        <v>1.760712448045744E-29</v>
+      </c>
+      <c r="Q12" s="44"/>
+    </row>
+    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="32">
+        <v>159.38</v>
+      </c>
+      <c r="D13" s="32">
+        <v>68.3</v>
+      </c>
+      <c r="E13" s="27">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F13" s="33">
+        <v>3.6572999999999999E-8</v>
+      </c>
+      <c r="G13" s="33">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="H13" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="39">
+        <v>4.43</v>
+      </c>
+      <c r="K13" s="39">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L13" s="42">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="M13" s="29">
+        <f t="shared" si="0"/>
+        <v>1.9634954087500001</v>
+      </c>
+      <c r="N13" s="43">
         <f>3.3492*24*3600</f>
         <v>289370.88</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O13" s="31">
         <f t="shared" si="1"/>
         <v>2.3953591342708707E-6</v>
       </c>
-      <c r="P11" s="29">
-        <f>F11/(6.022E+23*J11/K11)/L11</f>
-        <v>2.9216534713029442E-30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="30">
-        <v>159.38</v>
-      </c>
-      <c r="D12" s="30">
-        <v>68.3</v>
-      </c>
-      <c r="E12" s="25">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F12" s="31">
-        <v>3.83901E-8</v>
-      </c>
-      <c r="G12" s="31">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="H12" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I12" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="J12" s="26">
-        <v>4.43</v>
-      </c>
-      <c r="K12" s="26">
-        <v>46.951799999999999</v>
-      </c>
-      <c r="L12" s="27">
-        <v>7.4399999999999994E-2</v>
-      </c>
-      <c r="M12" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9634954087500001</v>
-      </c>
-      <c r="N12" s="50">
-        <f>3.3492*24*3600</f>
-        <v>289370.88</v>
-      </c>
-      <c r="O12" s="29">
-        <f t="shared" si="1"/>
-        <v>2.3953591342708707E-6</v>
-      </c>
-      <c r="P12" s="29">
-        <f t="shared" si="2"/>
-        <v>9.0814265969195732E-30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="30">
-        <v>1312.12</v>
-      </c>
-      <c r="D13" s="30">
-        <v>100.1</v>
-      </c>
-      <c r="E13" s="34">
-        <v>9944835104.503521</v>
-      </c>
-      <c r="F13" s="31">
-        <v>1.07354E-7</v>
-      </c>
-      <c r="G13" s="31">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H13" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I13" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="J13" s="24">
-        <v>4.43</v>
-      </c>
-      <c r="K13" s="24">
-        <v>47.947899999999997</v>
-      </c>
-      <c r="L13" s="35">
-        <v>0.73719999999999997</v>
-      </c>
-      <c r="M13" s="28">
-        <f t="shared" si="0"/>
-        <v>1.9634954087500001</v>
-      </c>
-      <c r="N13" s="51">
-        <f>43.67*3600</f>
-        <v>157212</v>
-      </c>
-      <c r="O13" s="29">
-        <f t="shared" si="1"/>
-        <v>4.4089966452942525E-6</v>
-      </c>
-      <c r="P13" s="29">
-        <f t="shared" si="2"/>
-        <v>2.6173271957228483E-30</v>
+      <c r="P13" s="31">
+        <f>F13/(6.022E+23*J13/K13)/L13</f>
+        <v>8.8202192853974607E-30</v>
+      </c>
+      <c r="Q13" s="30">
+        <v>8200</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C14" s="21">
-        <v>1761.9</v>
+        <v>889.27700000000004</v>
       </c>
       <c r="D14" s="21">
-        <v>0.05</v>
+        <v>99.983999999999995</v>
       </c>
       <c r="E14" s="16">
         <v>9944835104.503521</v>
       </c>
       <c r="F14" s="22">
-        <v>5.3777699999999997E-9</v>
+        <v>1.3664799999999999E-8</v>
       </c>
       <c r="G14" s="22">
-        <v>3.2000000000000002E-3</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="H14" s="15">
         <v>2.5</v>
@@ -1384,260 +1406,371 @@
       <c r="I14" s="15">
         <v>0.1</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="17">
         <v>4.43</v>
       </c>
       <c r="K14" s="17">
-        <v>48.947899999999997</v>
+        <v>47.866999999999997</v>
       </c>
       <c r="L14" s="18">
-        <v>5.4100000000000002E-2</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="M14" s="19">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N14" s="48">
-        <f>57.18*60</f>
-        <v>3430.8</v>
+      <c r="N14" s="36">
+        <v>7239456.0000000009</v>
       </c>
       <c r="O14" s="20">
         <f t="shared" si="1"/>
-        <v>2.0203660388247639E-4</v>
+        <v>9.5745755012531324E-8</v>
       </c>
       <c r="P14" s="20">
         <f t="shared" si="2"/>
-        <v>1.8238727961479583E-30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="21" t="s">
+        <v>3.2955057690399804E-30</v>
+      </c>
+      <c r="Q14" s="44"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="32">
         <v>1312.12</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="32">
         <v>100.1</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="26">
         <v>9944835104.503521</v>
       </c>
-      <c r="F15" s="22">
-        <v>9.1444600000000005E-10</v>
-      </c>
-      <c r="G15" s="22">
-        <v>7.3000000000000001E-3</v>
-      </c>
-      <c r="H15" s="15">
+      <c r="F15" s="33">
+        <v>1.01775E-7</v>
+      </c>
+      <c r="G15" s="33">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="H15" s="25">
         <v>2.5</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="25">
         <v>0.1</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="25">
         <v>4.43</v>
       </c>
-      <c r="K15" s="17">
-        <v>48.947899999999997</v>
-      </c>
-      <c r="L15" s="18">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="M15" s="19">
+      <c r="K15" s="39">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L15" s="28">
+        <v>0.73719999999999997</v>
+      </c>
+      <c r="M15" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N15" s="49">
+      <c r="N15" s="41">
         <f>43.67*3600</f>
         <v>157212</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="31">
         <f t="shared" si="1"/>
         <v>4.4089966452942525E-6</v>
       </c>
-      <c r="P15" s="20">
+      <c r="P15" s="31">
         <f t="shared" si="2"/>
-        <v>3.101347180980808E-31</v>
+        <v>2.4771226855629042E-30</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>8200</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="30">
-        <v>511</v>
-      </c>
-      <c r="D16" s="30">
-        <v>195.66</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="A16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="21">
+        <v>159.38</v>
+      </c>
+      <c r="D16" s="21">
+        <v>68.3</v>
+      </c>
+      <c r="E16" s="16">
         <v>9944835104.503521</v>
       </c>
-      <c r="F16" s="31">
-        <v>8.4934299999999998E-7</v>
-      </c>
-      <c r="G16" s="31">
-        <v>4.3E-3</v>
-      </c>
-      <c r="H16" s="24">
+      <c r="F16" s="22">
+        <v>7.0414699999999996E-8</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1.9E-2</v>
+      </c>
+      <c r="H16" s="15">
         <v>2.5</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="15">
         <v>0.1</v>
       </c>
-      <c r="J16" s="26">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="K16" s="23">
-        <v>62.929600000000001</v>
-      </c>
-      <c r="L16" s="32">
-        <v>0.69169999999999998</v>
-      </c>
-      <c r="M16" s="28">
+      <c r="J16" s="17">
+        <v>4.43</v>
+      </c>
+      <c r="K16" s="17">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L16" s="23">
+        <v>0.73719999999999997</v>
+      </c>
+      <c r="M16" s="19">
+        <f t="shared" ref="M16" si="6">3.141592654*H16^2*I16</f>
+        <v>1.9634954087500001</v>
+      </c>
+      <c r="N16" s="36">
+        <f>3.3492*24*3600</f>
+        <v>289370.88</v>
+      </c>
+      <c r="O16" s="20">
+        <f t="shared" ref="O16" si="7">0.6931471806/N16</f>
+        <v>2.3953591342708707E-6</v>
+      </c>
+      <c r="P16" s="20">
+        <f>F16/(6.022E+23*J16/K16)/L16</f>
+        <v>1.7138378852086094E-30</v>
+      </c>
+      <c r="Q16" s="44"/>
+    </row>
+    <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="21">
+        <v>1312.12</v>
+      </c>
+      <c r="D17" s="21">
+        <v>100.1</v>
+      </c>
+      <c r="E17" s="16">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F17" s="22">
+        <v>3.2979399999999999E-9</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="H17" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="14">
+        <v>4.43</v>
+      </c>
+      <c r="K17" s="14">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="L17" s="18">
+        <v>5.4100000000000002E-2</v>
+      </c>
+      <c r="M17" s="19">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N17" s="37">
+        <f>43.67*3600</f>
+        <v>157212</v>
+      </c>
+      <c r="O17" s="20">
+        <f t="shared" si="1"/>
+        <v>4.4089966452942525E-6</v>
+      </c>
+      <c r="P17" s="20">
+        <f t="shared" si="2"/>
+        <v>1.0937982323466035E-30</v>
+      </c>
+      <c r="Q17" s="44"/>
+    </row>
+    <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="32">
+        <v>511</v>
+      </c>
+      <c r="D18" s="32">
+        <v>195.66</v>
+      </c>
+      <c r="E18" s="27">
+        <v>9944835104.503521</v>
+      </c>
+      <c r="F18" s="33">
+        <v>7.9725600000000003E-7</v>
+      </c>
+      <c r="G18" s="33">
+        <v>1.37E-2</v>
+      </c>
+      <c r="H18" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="39">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="K18" s="24">
+        <v>63.545999999999999</v>
+      </c>
+      <c r="L18" s="40">
+        <v>0.69169999999999998</v>
+      </c>
+      <c r="M18" s="29">
+        <f t="shared" si="0"/>
+        <v>1.9634954087500001</v>
+      </c>
+      <c r="N18" s="35">
         <f>9.673*60</f>
         <v>580.38</v>
       </c>
-      <c r="O16" s="29">
+      <c r="O18" s="31">
         <f t="shared" si="1"/>
         <v>1.1942988741858783E-3</v>
       </c>
-      <c r="P16" s="29">
+      <c r="P18" s="31">
         <f t="shared" si="2"/>
-        <v>1.4320940704440049E-29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="30">
+        <v>1.3574363609995E-29</v>
+      </c>
+      <c r="Q18" s="30">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="32">
         <v>511</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D19" s="32">
         <v>21.65</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E19" s="27">
         <v>9944835104.503521</v>
       </c>
-      <c r="F17" s="31">
-        <v>6.81613E-7</v>
-      </c>
-      <c r="G17" s="31">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H17" s="24">
+      <c r="F19" s="33">
+        <v>6.4088600000000001E-7</v>
+      </c>
+      <c r="G19" s="33">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="H19" s="25">
         <v>2.5</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I19" s="25">
         <v>0.1</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J19" s="39">
         <v>8.9600000000000009</v>
       </c>
-      <c r="K17" s="23">
-        <v>64.927800000000005</v>
-      </c>
-      <c r="L17" s="32">
+      <c r="K19" s="24">
+        <v>63.545999999999999</v>
+      </c>
+      <c r="L19" s="40">
         <v>0.30830000000000002</v>
       </c>
-      <c r="M17" s="28">
+      <c r="M19" s="29">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N19" s="35">
         <f>12.701*3600</f>
         <v>45723.6</v>
       </c>
-      <c r="O17" s="29">
+      <c r="O19" s="31">
         <f t="shared" si="1"/>
         <v>1.515950582631289E-5</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P19" s="31">
         <f t="shared" si="2"/>
-        <v>2.6603958818106171E-29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="M18"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I22" s="6"/>
+        <v>2.4481990072108824E-29</v>
+      </c>
+      <c r="Q19" s="30">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="M20"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="L25">
-        <f>960+780+60+540</f>
-        <v>2340</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <f>300+450+60+420+60+750+60+1000+60+1350+60+5000+60+8200+60</f>
+        <v>17890</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
@@ -1712,6 +1845,14 @@
     <row r="50" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>